<commit_message>
update compiled data, filenames
</commit_message>
<xml_diff>
--- a/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-13.xlsx
+++ b/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-13.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Alpha</t>
   </si>
@@ -90,9 +90,6 @@
     <t>15-genes_28-edges_db5_Sigmoid_estimation_missing-values_fixP-fixb.xlsx</t>
   </si>
   <si>
-    <t>15-genes_28-edges_db5_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
-  </si>
-  <si>
     <t>15-genes_28-edges_db5_Sigmoid_estimation_missing-values_L-curve_no-GLN3-data.xlsx</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>15-genes_28-edges_db5_Sigmoid_estimation_missing-values_L-curve_no-GLN3-ZAP1-HAP4-HMO1-data.xlsx</t>
   </si>
   <si>
-    <t>15-genes_28-edges_db5_Sigmoid_estimation_no-missing-values_L-curve.xlsx</t>
-  </si>
-  <si>
     <t>15-genes_28-edges_db5-random7-fam_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
   </si>
   <si>
@@ -127,6 +121,39 @@
   </si>
   <si>
     <t>L-curve ID</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random2_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random3_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random9_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random12-fam_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random15_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random16-fam_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5-random31_Sigmoid_estimation_missing-values_L-curve.xlsx</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5_Sigmoid_estimation_no-missing-values_L-curve.xlsx SEA120-14</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5_Sigmoid_estimation_missing-values_L-curve.xlsx SEA120-14</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5_Sigmoid_estimation_no-missing-values_L-curve.xlsx SEA120-15</t>
+  </si>
+  <si>
+    <t>15-genes_28-edges_db5_Sigmoid_estimation_missing-values_L-curve.xlsx SEA120-15</t>
   </si>
 </sst>
 </file>
@@ -443,11 +470,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -456,7 +481,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -467,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -475,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -483,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -491,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -499,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -507,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -515,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -523,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -531,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,7 +564,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -547,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -555,7 +580,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -563,7 +588,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -571,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -579,7 +604,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -587,7 +612,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -595,7 +620,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -603,7 +628,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -611,7 +636,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -619,7 +644,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -627,7 +652,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -635,7 +660,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -643,7 +668,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -651,7 +676,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -659,7 +684,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -667,7 +692,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -675,7 +700,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -683,7 +708,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -691,7 +716,79 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>